<commit_message>
Update BSides22 Project Summary.xlsx
</commit_message>
<xml_diff>
--- a/Docs/BSides22 Project Summary.xlsx
+++ b/Docs/BSides22 Project Summary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{EAA2DF16-169E-4ED2-A65E-34806AA77400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD39E83C-A050-474F-BF6E-66F9B4E766AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9295E66-D960-43D6-B7F9-96091E7DBE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6045" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Summary" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="175">
   <si>
     <t>Project Name</t>
   </si>
@@ -557,6 +557,9 @@
   </si>
   <si>
     <t>These are Adjustable Values</t>
+  </si>
+  <si>
+    <t>Learn to Solder Kits</t>
   </si>
 </sst>
 </file>
@@ -2461,10 +2464,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230ECA56-04B2-4271-9B6D-69C62BBA135C}">
-  <dimension ref="B1:P37"/>
+  <dimension ref="B1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2486,8 +2489,8 @@
     <col min="16" max="16" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="127" t="s">
         <v>147</v>
       </c>
@@ -2505,7 +2508,7 @@
       </c>
       <c r="L2" s="120"/>
     </row>
-    <row r="3" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="79" t="s">
         <v>148</v>
       </c>
@@ -2524,7 +2527,7 @@
         <v>39</v>
       </c>
       <c r="I3" s="77">
-        <f>I27</f>
+        <f>I28</f>
         <v>600</v>
       </c>
       <c r="K3" s="50" t="s">
@@ -2532,12 +2535,12 @@
       </c>
       <c r="L3" s="48"/>
     </row>
-    <row r="4" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="81" t="s">
         <v>149</v>
       </c>
       <c r="C4" s="82">
-        <f>C29</f>
+        <f>C30</f>
         <v>515</v>
       </c>
       <c r="E4" s="56"/>
@@ -2546,11 +2549,11 @@
         <v>51</v>
       </c>
       <c r="L4" s="91">
-        <f>L17</f>
-        <v>12977.66</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <f>L18</f>
+        <v>13427.66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="K5" s="51" t="s">
         <v>161</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="125" t="s">
         <v>40</v>
       </c>
@@ -2576,10 +2579,10 @@
       </c>
       <c r="L6" s="92">
         <f>L4-L5</f>
-        <v>8977.66</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+        <v>9427.66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B7" s="34" t="s">
         <v>43</v>
       </c>
@@ -2601,12 +2604,12 @@
         <v>149.57</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B8" s="34" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="42">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>44</v>
@@ -2618,10 +2621,10 @@
         <v>44</v>
       </c>
       <c r="I8" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B9" s="34" t="s">
         <v>146</v>
       </c>
@@ -2641,12 +2644,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B10" s="34" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="86">
-        <f>D32</f>
+        <f>D33</f>
         <v>374.57999999999993</v>
       </c>
       <c r="E10" s="34" t="s">
@@ -2659,16 +2662,16 @@
         <v>46</v>
       </c>
       <c r="I10" s="86">
-        <f>J30</f>
+        <f>J31</f>
         <v>288.3</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B11" s="34" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="86">
-        <f>D29</f>
+        <f>D30</f>
         <v>1034.67</v>
       </c>
       <c r="E11" s="34" t="s">
@@ -2681,11 +2684,11 @@
         <v>48</v>
       </c>
       <c r="I11" s="86">
-        <f>J27</f>
+        <f>J28</f>
         <v>320.45</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B12" s="35" t="s">
         <v>79</v>
       </c>
@@ -2703,12 +2706,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B13" s="35" t="s">
         <v>80</v>
       </c>
       <c r="C13" s="60">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>80</v>
@@ -2723,12 +2726,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B14" s="35" t="s">
         <v>163</v>
       </c>
       <c r="C14" s="60">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>163</v>
@@ -2743,344 +2746,356 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B15" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="60">
+        <v>400</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="60"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="60"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="60">
+      <c r="C16" s="60">
         <v>0</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E16" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="F15" s="60">
+      <c r="F16" s="60">
         <v>0</v>
       </c>
-      <c r="H15" s="35" t="s">
+      <c r="H16" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="I15" s="60">
+      <c r="I16" s="60">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="35" t="s">
+    <row r="17" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C17" s="39">
         <f>'ConBadge BOM'!J32</f>
         <v>2248.5</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E17" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F17" s="39">
         <f>'KidsBadge BOM'!J29</f>
         <v>0</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H17" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I17" s="39">
         <f>'SAO BOM'!J14</f>
         <v>240</v>
       </c>
-      <c r="O16" s="53"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="36" t="s">
+      <c r="O17" s="53"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="40">
-        <f>SUM(C7:C16)</f>
-        <v>11268.380000000001</v>
-      </c>
-      <c r="E17" s="36" t="s">
+      <c r="C18" s="40">
+        <f>SUM(C7:C17)</f>
+        <v>11618.380000000001</v>
+      </c>
+      <c r="E18" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="40">
-        <f>SUM(F7:F16)</f>
+      <c r="F18" s="40">
+        <f>SUM(F7:F17)</f>
         <v>710.95999999999992</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="H18" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="40">
-        <f>SUM(I7:I16)</f>
-        <v>998.31999999999994</v>
-      </c>
-      <c r="K17" s="28" t="s">
+      <c r="I18" s="40">
+        <f>SUM(I7:I17)</f>
+        <v>1098.32</v>
+      </c>
+      <c r="K18" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="27">
-        <f>C17+F17+I17</f>
-        <v>12977.66</v>
-      </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="O18" s="53"/>
-      <c r="P18" s="55"/>
+      <c r="L18" s="27">
+        <f>C18+F18+I18</f>
+        <v>13427.66</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="1"/>
     </row>
     <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="26" t="s">
+      <c r="O19" s="53"/>
+      <c r="P19" s="55"/>
+    </row>
+    <row r="20" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="29">
-        <f>C17 / (C3)</f>
-        <v>30.049013333333335</v>
-      </c>
-      <c r="E19" s="26" t="s">
+      <c r="C20" s="29">
+        <f>C18 / (C3)</f>
+        <v>30.982346666666668</v>
+      </c>
+      <c r="E20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="29">
-        <f>F17/F3</f>
+      <c r="F20" s="29">
+        <f>F18/F3</f>
         <v>17.773999999999997</v>
       </c>
-      <c r="H19" s="26" t="s">
+      <c r="H20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="29">
-        <f>I17/I3</f>
-        <v>1.6638666666666666</v>
-      </c>
-      <c r="L19" s="3"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="H20" s="56"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="29">
+        <f>I18/I3</f>
+        <v>1.8305333333333331</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="3"/>
     </row>
     <row r="21" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="119" t="s">
+      <c r="H21" s="56"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="119" t="s">
         <v>158</v>
       </c>
-      <c r="C21" s="121"/>
-      <c r="D21" s="120"/>
-      <c r="H21" s="122" t="s">
+      <c r="C22" s="121"/>
+      <c r="D22" s="120"/>
+      <c r="H22" s="122" t="s">
         <v>159</v>
       </c>
-      <c r="I21" s="123"/>
-      <c r="J21" s="124"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B22" s="100" t="s">
+      <c r="I22" s="123"/>
+      <c r="J22" s="124"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B23" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="101">
+      <c r="C23" s="101">
         <f>'Project Summary'!C7</f>
         <v>375</v>
       </c>
-      <c r="D22" s="99">
+      <c r="D23" s="99">
         <v>577.08000000000004</v>
       </c>
-      <c r="H22" s="97" t="s">
+      <c r="H23" s="97" t="s">
         <v>152</v>
       </c>
-      <c r="I22" s="98">
+      <c r="I23" s="98">
         <v>400</v>
       </c>
-      <c r="J22" s="99">
+      <c r="J23" s="99">
         <v>175.39</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B23" s="79" t="s">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B24" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <f>'Project Summary'!E7</f>
         <v>35</v>
       </c>
-      <c r="D23" s="83">
+      <c r="D24" s="83">
         <v>87.97</v>
       </c>
-      <c r="H23" s="95" t="s">
+      <c r="H24" s="95" t="s">
         <v>153</v>
       </c>
-      <c r="I23" s="90">
+      <c r="I24" s="90">
         <v>50</v>
       </c>
-      <c r="J23" s="83">
+      <c r="J24" s="83">
         <v>25.97</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B24" s="79" t="s">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B25" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <f>'Project Summary'!F7</f>
         <v>10</v>
       </c>
-      <c r="D24" s="83">
+      <c r="D25" s="83">
         <v>108.71</v>
       </c>
-      <c r="H24" s="95" t="s">
+      <c r="H25" s="95" t="s">
         <v>154</v>
       </c>
-      <c r="I24" s="90">
+      <c r="I25" s="90">
         <v>50</v>
       </c>
-      <c r="J24" s="83">
+      <c r="J25" s="83">
         <v>77.03</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B25" s="79" t="s">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B26" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C26" s="2">
         <f>'Project Summary'!G7</f>
         <v>30</v>
       </c>
-      <c r="D25" s="83">
+      <c r="D26" s="83">
         <v>63.31</v>
       </c>
-      <c r="H25" s="95" t="s">
+      <c r="H26" s="95" t="s">
         <v>155</v>
-      </c>
-      <c r="I25" s="90">
-        <v>50</v>
-      </c>
-      <c r="J25" s="83">
-        <v>21.29</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B26" s="79" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="2">
-        <v>10</v>
-      </c>
-      <c r="D26" s="83">
-        <v>39.47</v>
-      </c>
-      <c r="H26" s="95" t="s">
-        <v>156</v>
       </c>
       <c r="I26" s="90">
         <v>50</v>
       </c>
       <c r="J26" s="83">
+        <v>21.29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="B27" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="2">
+        <v>10</v>
+      </c>
+      <c r="D27" s="83">
+        <v>39.47</v>
+      </c>
+      <c r="H27" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="I27" s="90">
+        <v>50</v>
+      </c>
+      <c r="J27" s="83">
         <v>20.77</v>
       </c>
     </row>
-    <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="79" t="s">
+    <row r="28" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B28" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C28" s="2">
         <f>'Project Summary'!I7</f>
         <v>30</v>
       </c>
-      <c r="D27" s="83">
+      <c r="D28" s="83">
         <v>94.82</v>
       </c>
-      <c r="H27" s="96" t="s">
+      <c r="H28" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="I27" s="8">
-        <f>SUM(I22:I26)</f>
+      <c r="I28" s="8">
+        <f>SUM(I23:I27)</f>
         <v>600</v>
       </c>
-      <c r="J27" s="87">
-        <f>SUM(J22:J26)</f>
+      <c r="J28" s="87">
+        <f>SUM(J23:J27)</f>
         <v>320.45</v>
       </c>
     </row>
-    <row r="28" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="81" t="s">
+    <row r="29" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C29" s="8">
         <f>'Project Summary'!H7</f>
         <v>25</v>
       </c>
-      <c r="D28" s="84">
+      <c r="D29" s="84">
         <v>63.31</v>
       </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="94" t="s">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B30" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="C29" s="41">
-        <f>SUM(C22:C28)</f>
+      <c r="C30" s="41">
+        <f>SUM(C23:C29)</f>
         <v>515</v>
       </c>
-      <c r="D29" s="93">
-        <f>SUM(D22:D28)</f>
+      <c r="D30" s="93">
+        <f>SUM(D23:D29)</f>
         <v>1034.67</v>
       </c>
-      <c r="I29" s="88" t="s">
+      <c r="I30" s="88" t="s">
         <v>165</v>
       </c>
-      <c r="J29" s="48">
+      <c r="J30" s="48">
         <f>293.7+315.05</f>
         <v>608.75</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="I30" s="89" t="s">
+    <row r="31" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="I31" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="J30" s="87">
-        <f>J29-J27</f>
+      <c r="J31" s="87">
+        <f>J30-J28</f>
         <v>288.3</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="C31" s="88" t="s">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="C32" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="D31" s="48">
+      <c r="D32" s="48">
         <v>1409.25</v>
       </c>
     </row>
-    <row r="32" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C32" s="89" t="s">
+    <row r="33" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C33" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="85">
-        <f>D31-D29</f>
+      <c r="D33" s="85">
+        <f>D32-D30</f>
         <v>374.57999999999993</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="34" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="22" t="s">
+    <row r="34" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="35" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B35" s="23" t="s">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B36" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B36" s="24" t="s">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B37" s="24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B37" s="25" t="s">
+    <row r="38" spans="2:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B38" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="H37" s="56"/>
-      <c r="I37" s="55"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="H22:J22"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="H6:I6"/>

</xml_diff>